<commit_message>
added a case for the deleted watermark
</commit_message>
<xml_diff>
--- a/voter_data.xlsx
+++ b/voter_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2363,42 +2363,6 @@
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>SNEHAL AMOL WAJARE</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>VIY RANBNARE</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>FTHR</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
-        <v>33</v>
-      </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
enhanced the images and cropped in two parts
</commit_message>
<xml_diff>
--- a/voter_data.xlsx
+++ b/voter_data.xlsx
@@ -812,7 +812,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PRALHAD YADAV</t>
+          <t>PRALHADYADAV</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1131,7 +1131,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>RAJASHRI KASAR</t>
+          <t>RAJASHRIKASAR</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>PRAJAKTA PRASADPALKAR</t>
+          <t>PRAJAKTA PRASAD PALKAR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ASHOK CHAUHAN</t>
+          <t>ASHOKCHAUHAN</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ASHOKCHAUHAN</t>
+          <t>ASHOK CHAUHAN</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1947,11 +1947,7 @@
       <c r="E40" t="n">
         <v>42</v>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
           <t>11A</t>
@@ -1971,7 +1967,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>KRANTIASHOK CHAUHAN</t>
+          <t>KRANTI ASHOK CHAUHAN</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">

</xml_diff>